<commit_message>
merge_teams is now more protected
</commit_message>
<xml_diff>
--- a/merge.xlsx
+++ b/merge.xlsx
@@ -20,11 +20,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="82">
   <si>
     <t xml:space="preserve">Index</t>
   </si>
   <si>
+    <t xml:space="preserve">created</t>
+  </si>
+  <si>
     <t xml:space="preserve">bracket team</t>
   </si>
   <si>
@@ -37,7 +40,13 @@
     <t xml:space="preserve">fixed stats team</t>
   </si>
   <si>
+    <t xml:space="preserve">2024-07-28 10:07:59</t>
+  </si>
+  <si>
     <t xml:space="preserve">Akron</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve">Alabama</t>
@@ -266,7 +275,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,6 +305,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -347,13 +362,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -548,17 +567,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E63" activeCellId="0" sqref="E63"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.82"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -577,18 +596,24 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -597,12 +622,15 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -611,12 +639,15 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -628,9 +659,12 @@
         <v>8</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -639,12 +673,15 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -653,12 +690,15 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -667,12 +707,15 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -681,12 +724,15 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -695,12 +741,15 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -709,12 +758,15 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -723,12 +775,15 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -737,12 +792,15 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -751,12 +809,15 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -765,12 +826,15 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -779,12 +843,15 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -793,12 +860,15 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -807,12 +877,15 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -821,16 +894,19 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="0" t="n">
         <v>67</v>
       </c>
-      <c r="E19" s="0" t="s">
-        <v>24</v>
+      <c r="F19" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -838,12 +914,15 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -852,12 +931,15 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -866,12 +948,15 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -880,12 +965,15 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -894,12 +982,15 @@
         <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="D24" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -908,12 +999,15 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -922,12 +1016,15 @@
         <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E26" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -936,12 +1033,15 @@
         <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D27" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -950,12 +1050,15 @@
         <v>27</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -964,12 +1067,15 @@
         <v>28</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D29" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -978,12 +1084,15 @@
         <v>29</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="D30" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -992,12 +1101,15 @@
         <v>30</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="D31" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E31" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1006,12 +1118,15 @@
         <v>31</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="D32" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E32" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1020,12 +1135,15 @@
         <v>32</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="D33" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="E33" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1034,12 +1152,15 @@
         <v>33</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="D34" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" s="0" t="n">
         <v>82</v>
       </c>
     </row>
@@ -1048,12 +1169,15 @@
         <v>34</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D35" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1062,12 +1186,15 @@
         <v>35</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="D36" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E36" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1076,12 +1203,15 @@
         <v>36</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="D37" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E37" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1090,12 +1220,15 @@
         <v>37</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="D38" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E38" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1104,12 +1237,15 @@
         <v>38</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D39" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E39" s="0" t="n">
         <v>82</v>
       </c>
     </row>
@@ -1118,12 +1254,15 @@
         <v>39</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="D40" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="E40" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1132,12 +1271,15 @@
         <v>40</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="D41" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E41" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1146,12 +1288,15 @@
         <v>41</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="D42" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="E42" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1160,12 +1305,15 @@
         <v>42</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D43" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E43" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1174,12 +1322,15 @@
         <v>43</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D44" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="E44" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1188,12 +1339,15 @@
         <v>44</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="D45" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E45" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1202,12 +1356,15 @@
         <v>45</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="D46" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E46" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1216,12 +1373,15 @@
         <v>46</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D47" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E47" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1230,12 +1390,15 @@
         <v>47</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="D48" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E48" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1244,12 +1407,15 @@
         <v>48</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="D49" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E49" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1258,12 +1424,15 @@
         <v>49</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D50" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E50" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1272,12 +1441,15 @@
         <v>50</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="D51" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="E51" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1286,12 +1458,15 @@
         <v>51</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="D52" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E52" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1300,12 +1475,15 @@
         <v>52</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="D53" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E53" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1314,12 +1492,15 @@
         <v>53</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="D54" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E54" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1328,12 +1509,15 @@
         <v>54</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="D55" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="E55" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1342,12 +1526,15 @@
         <v>55</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="D56" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E56" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1356,12 +1543,15 @@
         <v>56</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="D57" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="E57" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1370,12 +1560,15 @@
         <v>57</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>65</v>
+        <v>8</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="D58" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="E58" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1384,12 +1577,15 @@
         <v>58</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>66</v>
+        <v>8</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="D59" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E59" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1398,12 +1594,15 @@
         <v>59</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="D60" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="E60" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1412,16 +1611,19 @@
         <v>60</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>68</v>
+        <v>8</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="D61" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E61" s="0" t="n">
         <v>57</v>
       </c>
-      <c r="E61" s="0" t="s">
-        <v>70</v>
+      <c r="F61" s="2" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1429,12 +1631,15 @@
         <v>61</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="D62" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="E62" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1443,12 +1648,15 @@
         <v>62</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="D63" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E63" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1457,12 +1665,15 @@
         <v>63</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>73</v>
+        <v>8</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="D64" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="E64" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1471,12 +1682,15 @@
         <v>64</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="D65" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="E65" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1485,12 +1699,15 @@
         <v>65</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>75</v>
+        <v>8</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="D66" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="E66" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1499,12 +1716,15 @@
         <v>66</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>76</v>
+        <v>8</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="D67" s="0" t="n">
+        <v>79</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="E67" s="0" t="n">
         <v>77</v>
       </c>
     </row>
@@ -1513,12 +1733,15 @@
         <v>67</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>69</v>
+        <v>8</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="D68" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="D68" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E68" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1527,12 +1750,15 @@
         <v>68</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>78</v>
+        <v>8</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="D69" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="E69" s="0" t="n">
         <v>100</v>
       </c>
     </row>

</xml_diff>